<commit_message>
add result for 20 degree heeling angle
</commit_message>
<xml_diff>
--- a/Simulation/Sail.xlsx
+++ b/Simulation/Sail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Foil</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>F (N)</t>
+  </si>
+  <si>
+    <t>20°</t>
   </si>
 </sst>
 </file>
@@ -165,10 +168,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -179,15 +178,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Feuil1!$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v bateau (kts)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>heeling 0°</c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
@@ -196,10 +187,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.79439848103607935</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2468982116196186</c:v>
+                  <c:v>2.284057960812651</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4.4937964232392371</c:v>
@@ -245,6 +236,68 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.8876923435786983</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>heeling 20°</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$E$26:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.80270576191234067</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2776943598307287</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5847185819595619</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5485414043341548</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9917519666762349</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.134290528811785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$A$26:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.19438461717893493</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63175000583153851</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0691153944841421</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5064807831367457</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9438461717893492</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.915769257684024</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -259,11 +312,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137427712"/>
-        <c:axId val="137428288"/>
+        <c:axId val="137558784"/>
+        <c:axId val="137559360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137427712"/>
+        <c:axId val="137558784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -273,12 +326,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137428288"/>
+        <c:crossAx val="137559360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137428288"/>
+        <c:axId val="137559360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -289,7 +342,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137427712"/>
+        <c:crossAx val="137558784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -633,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,15 +878,15 @@
         <v>0.1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" ref="D15:D21" si="0">SQRT(C15/(0.5*rho*len*h*$B$10))</f>
-        <v>0</v>
+        <v>0.4086735321781248</v>
       </c>
       <c r="E15" s="4">
         <f>D15/0.514444</f>
-        <v>0</v>
+        <v>0.79439848103607935</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -845,15 +898,15 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C16">
-        <v>0.02</v>
+        <v>2.0667000000000001E-2</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" si="0"/>
-        <v>1.1559033035784432</v>
+        <v>1.1750199135923034</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" ref="E16:E21" si="2">D16/0.514444</f>
-        <v>2.2468982116196186</v>
+        <v>2.284057960812651</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -955,6 +1008,159 @@
         <f t="shared" si="2"/>
         <v>13.481389269717711</v>
       </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <f>B26/0.514444</f>
+        <v>0.19438461717893493</v>
+      </c>
+      <c r="B26">
+        <v>0.1</v>
+      </c>
+      <c r="C26">
+        <v>2.5525600000000002E-3</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" ref="D26:D32" si="3">SQRT(C26/(0.5*rho*len*h*$B$10))</f>
+        <v>0.41294716298123219</v>
+      </c>
+      <c r="E26" s="4">
+        <f>D26/0.514444</f>
+        <v>0.80270576191234067</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <f t="shared" ref="A27:A32" si="4">B27/0.514444</f>
+        <v>0.63175000583153851</v>
+      </c>
+      <c r="B27">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="C27">
+        <v>2.0552000000000001E-2</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="3"/>
+        <v>1.1717461972487595</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" ref="E27:E32" si="5">D27/0.514444</f>
+        <v>2.2776943598307287</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0691153944841421</v>
+      </c>
+      <c r="B28">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C28">
+        <v>8.3269999999999997E-2</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="3"/>
+        <v>2.3585809661776049</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="5"/>
+        <v>4.5847185819595619</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <f t="shared" si="4"/>
+        <v>1.5064807831367457</v>
+      </c>
+      <c r="B29">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="C29">
+        <v>0.22572999999999999</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" si="3"/>
+        <v>3.8833018342112799</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="5"/>
+        <v>7.5485414043341548</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <f t="shared" si="4"/>
+        <v>1.9438461717893492</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0.39550000000000002</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="3"/>
+        <v>5.1401968487447895</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" si="5"/>
+        <v>9.9917519666762349</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <f t="shared" si="4"/>
+        <v>2.915769257684024</v>
+      </c>
+      <c r="B31">
+        <v>1.5</v>
+      </c>
+      <c r="C31">
+        <v>0.58330000000000004</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="3"/>
+        <v>6.2424129568040501</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="5"/>
+        <v>12.134290528811785</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add vacuum forming box plans
</commit_message>
<xml_diff>
--- a/Simulation/Sail.xlsx
+++ b/Simulation/Sail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>Foil</t>
   </si>
@@ -97,6 +97,54 @@
   </si>
   <si>
     <t>850g</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>épaisseur bois</t>
+  </si>
+  <si>
+    <t>planche haut/bas</t>
+  </si>
+  <si>
+    <t>planche gauche/droite</t>
+  </si>
+  <si>
+    <t>plaque bois</t>
+  </si>
+  <si>
+    <t>Cadre</t>
+  </si>
+  <si>
+    <t>chevauchement bois</t>
+  </si>
+  <si>
+    <t>baguette haut</t>
+  </si>
+  <si>
+    <t>baguette bas</t>
+  </si>
+  <si>
+    <t>qqt</t>
+  </si>
+  <si>
+    <t>vis longue</t>
+  </si>
+  <si>
+    <t>papillon</t>
+  </si>
+  <si>
+    <t>petites vis</t>
+  </si>
+  <si>
+    <t>Vacuum forming box</t>
+  </si>
+  <si>
+    <t>PS sheet</t>
   </si>
 </sst>
 </file>
@@ -315,6 +363,71 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>gite 20°</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$E$26:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.80270576191234067</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2776943598307287</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5847185819595619</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5485414043341548</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9917519666762349</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.134290528811785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$A$26:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.19438461717893493</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63175000583153851</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0691153944841421</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5064807831367457</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9438461717893492</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.915769257684024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -323,11 +436,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94668480"/>
-        <c:axId val="94669056"/>
+        <c:axId val="154148864"/>
+        <c:axId val="154149440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94668480"/>
+        <c:axId val="154148864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -337,12 +450,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94669056"/>
+        <c:crossAx val="154149440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94669056"/>
+        <c:axId val="154149440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -353,7 +466,239 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94668480"/>
+        <c:crossAx val="154148864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>700g</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$A$15:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.19438461717893493</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63175000583153851</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0691153944841421</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5064807831367457</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9438461717893492</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.915769257684024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8876923435786983</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$C$15:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0667000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>850g</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$A$36:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.19438461717893493</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63175000583153851</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0691153944841421</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5064807831367457</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9438461717893492</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.915769257684024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$C$36:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.7720000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1947999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4579999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27600999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.50819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6885</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="154151744"/>
+        <c:axId val="154152320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="154151744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154152320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="154152320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154151744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -402,6 +747,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -697,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,7 +1589,7 @@
         <v>2.7720000000000002E-3</v>
       </c>
       <c r="D36" s="5">
-        <f t="shared" ref="D36:D42" si="6">SQRT(C36/(0.5*rho*len*h*$B$10))</f>
+        <f t="shared" ref="D36:D41" si="6">SQRT(C36/(0.5*rho*len*h*$B$10))</f>
         <v>0.43033148291193524</v>
       </c>
       <c r="E36" s="4">
@@ -1224,7 +1599,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <f t="shared" ref="A37:A43" si="7">B37/0.514444</f>
+        <f t="shared" ref="A37:A41" si="7">B37/0.514444</f>
         <v>0.63175000583153851</v>
       </c>
       <c r="B37">
@@ -1238,7 +1613,7 @@
         <v>1.2108880210750839</v>
       </c>
       <c r="E37" s="4">
-        <f t="shared" ref="E37:E42" si="8">D37/0.514444</f>
+        <f t="shared" ref="E37:E41" si="8">D37/0.514444</f>
         <v>2.3537800442323826</v>
       </c>
     </row>
@@ -1329,6 +1704,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1339,14 +1724,158 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <f>B3-0.5</f>
+        <v>31.5</v>
+      </c>
+      <c r="C7">
+        <f>C3-0.5</f>
+        <v>19.5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <f>C7+B5/2</f>
+        <v>20.25</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <f>B7+B5/2</f>
+        <v>32.25</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <f>C3+C4*2</f>
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14">
+        <f>B3+B4*2</f>
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16">
+        <f>8+6</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>